<commit_message>
Database and error solved
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,21 @@
           <t>Name</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2/7/23</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>4/4/23</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>4/3/23</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -446,6 +461,21 @@
           <t>Sumit</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -453,6 +483,21 @@
           <t>Nigel</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -460,6 +505,21 @@
           <t>Abhay</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -467,6 +527,21 @@
           <t>Afzal</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -474,6 +549,21 @@
           <t>Prakhar</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -481,11 +571,41 @@
           <t>Avon</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
           <t>Kainaat</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Database Names from comparision of identified values
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,41 +436,44 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Roll No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>2/7/23</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>4/4/23</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>4/3/23</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>2/14/23</t>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>4/5/23</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Sumit</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>PRESENT</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>PRESENT</t>
@@ -486,18 +489,21 @@
           <t>PRESENT</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Nigel</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>PRESENT</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>PRESENT</t>
@@ -513,18 +519,21 @@
           <t>PRESENT</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Abhay</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>PRESENT</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>PRESENT</t>
@@ -540,18 +549,21 @@
           <t>PRESENT</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Afzal</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>PRESENT</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>PRESENT</t>
@@ -567,18 +579,21 @@
           <t>PRESENT</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Prakhar</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>PRESENT</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>PRESENT</t>
@@ -594,18 +609,21 @@
           <t>PRESENT</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Avon</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ABSENT</t>
-        </is>
-      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>ABSENT</t>
@@ -621,18 +639,21 @@
           <t>ABSENT</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Kainaat</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ABSENT</t>
-        </is>
-      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>ABSENT</t>
@@ -644,6 +665,11 @@
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>ABSENT</t>
         </is>

</xml_diff>